<commit_message>
added shocked excel file
</commit_message>
<xml_diff>
--- a/cge_variables.xlsx
+++ b/cge_variables.xlsx
@@ -2207,7 +2207,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2222,487 +2222,324 @@
       <c r="B1" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="n">
-        <v>2</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>CAP</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>AGR</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
+          <t>('CAP', 'AGR')</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>1135500.496578688</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>CAP</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>MIN</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
+          <t>('CAP', 'MIN')</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>131043.4885862961</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>CAP</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>MAN</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
+          <t>('CAP', 'MAN')</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>2283937.65102503</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CAP</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>ESW</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
+          <t>('CAP', 'ESW')</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>426893.2019172087</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>CAP</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>CON</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
+          <t>('CAP', 'CON')</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>744992.4177883761</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>CAP</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>WRT</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
+          <t>('CAP', 'WRT')</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
         <v>1787008.499114996</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CAP</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>TRS</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
+          <t>('CAP', 'TRS')</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
         <v>425529.1181899618</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CAP</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>AFS</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
+          <t>('CAP', 'AFS')</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
         <v>224861.258063752</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CAP</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>INF</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
+          <t>('CAP', 'INF')</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
         <v>316229.8417085022</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>CAP</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>FIN</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
+          <t>('CAP', 'FIN')</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
         <v>917723.7076114072</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CAP</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>REA</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
+          <t>('CAP', 'REA')</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
         <v>1029993.646087451</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>CAP</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>PBS</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
+          <t>('CAP', 'PBS')</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
         <v>418612.9897780325</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>CAP</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>PAD</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
+          <t>('CAP', 'PAD')</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
         <v>99793.11102378671</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>CAP</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>EDU</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
+          <t>('CAP', 'EDU')</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
         <v>162559.2634633618</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>CAP</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>HHS</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
+          <t>('CAP', 'HHS')</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
         <v>213874.0429722403</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>CAP</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>OTH</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
+          <t>('CAP', 'OTH')</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
         <v>265197.5242526537</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>LAB</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>AGR</t>
-        </is>
-      </c>
-      <c r="C18" t="n">
+          <t>('LAB', 'AGR')</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
         <v>580692</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>LAB</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>MIN</t>
-        </is>
-      </c>
-      <c r="C19" t="n">
+          <t>('LAB', 'MIN')</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
         <v>23593</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>LAB</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>MAN</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
+          <t>('LAB', 'MAN')</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
         <v>959036.53</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>LAB</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>ESW</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
+          <t>('LAB', 'ESW')</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
         <v>92438</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>LAB</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>CON</t>
-        </is>
-      </c>
-      <c r="C22" t="n">
+          <t>('LAB', 'CON')</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
         <v>576094</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>LAB</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>WRT</t>
-        </is>
-      </c>
-      <c r="C23" t="n">
+          <t>('LAB', 'WRT')</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
         <v>975807</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>LAB</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>TRS</t>
-        </is>
-      </c>
-      <c r="C24" t="n">
+          <t>('LAB', 'TRS')</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
         <v>241220</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>LAB</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>AFS</t>
-        </is>
-      </c>
-      <c r="C25" t="n">
+          <t>('LAB', 'AFS')</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
         <v>127419</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>LAB</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>INF</t>
-        </is>
-      </c>
-      <c r="C26" t="n">
+          <t>('LAB', 'INF')</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
         <v>156760</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>LAB</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>FIN</t>
-        </is>
-      </c>
-      <c r="C27" t="n">
+          <t>('LAB', 'FIN')</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
         <v>427069</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>LAB</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>REA</t>
-        </is>
-      </c>
-      <c r="C28" t="n">
+          <t>('LAB', 'REA')</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
         <v>56837</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>LAB</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>PBS</t>
-        </is>
-      </c>
-      <c r="C29" t="n">
+          <t>('LAB', 'PBS')</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
         <v>725200</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>LAB</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>PAD</t>
-        </is>
-      </c>
-      <c r="C30" t="n">
+          <t>('LAB', 'PAD')</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
         <v>612367</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>LAB</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>EDU</t>
-        </is>
-      </c>
-      <c r="C31" t="n">
+          <t>('LAB', 'EDU')</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
         <v>559598</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>LAB</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>HHS</t>
-        </is>
-      </c>
-      <c r="C32" t="n">
+          <t>('LAB', 'HHS')</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
         <v>84287</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>LAB</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>OTH</t>
-        </is>
-      </c>
-      <c r="C33" t="n">
+          <t>('LAB', 'OTH')</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
         <v>98666.46999999974</v>
       </c>
     </row>
@@ -3178,7 +3015,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:B257"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3193,488 +3030,2565 @@
       <c r="B1" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="n">
-        <v>2</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>CAP</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>AGR</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>1135500.496578688</v>
+          <t>('AGR', 'AGR')</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>996184.050494849</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>CAP</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>MIN</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>131043.4885862961</v>
+          <t>('AGR', 'MIN')</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>976.8286270496617</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>CAP</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>MAN</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>2283937.65102503</v>
+          <t>('AGR', 'MAN')</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1335493.450539227</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CAP</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>ESW</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>426893.2019172087</v>
+          <t>('AGR', 'ESW')</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>2112.539597468874</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>CAP</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>CON</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>744992.4177883761</v>
+          <t>('AGR', 'CON')</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>3120.123852353638</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>CAP</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>WRT</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>1787008.499114996</v>
+          <t>('AGR', 'WRT')</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>13906.41378521889</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CAP</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>TRS</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>425529.1181899618</v>
+          <t>('AGR', 'TRS')</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>790.3713158162036</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CAP</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>AFS</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>224861.258063752</v>
+          <t>('AGR', 'AFS')</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>8004.610860240749</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CAP</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>INF</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>316229.8417085022</v>
+          <t>('AGR', 'INF')</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>567.3164122969201</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>CAP</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>FIN</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>917723.7076114072</v>
+          <t>('AGR', 'FIN')</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>831.6523942152977</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CAP</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>REA</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>1029993.646087451</v>
+          <t>('AGR', 'REA')</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>994.4142883118851</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>CAP</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>PBS</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>418612.9897780325</v>
+          <t>('AGR', 'PBS')</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>2668.348360238089</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>CAP</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>PAD</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>99793.11102378671</v>
+          <t>('AGR', 'PAD')</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>2408.744516456872</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>CAP</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>EDU</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>162559.2634633618</v>
+          <t>('AGR', 'EDU')</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>887.2225417552854</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>CAP</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>HHS</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>213874.0429722403</v>
+          <t>('AGR', 'HHS')</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>769.1315417398619</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>CAP</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>OTH</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
-        <v>265197.5242526537</v>
+          <t>('AGR', 'OTH')</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>841.3175629623918</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>LAB</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>AGR</t>
-        </is>
-      </c>
-      <c r="C18" t="n">
-        <v>580692</v>
+          <t>('MIN', 'AGR')</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>43.99404506602389</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>LAB</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>MIN</t>
-        </is>
-      </c>
-      <c r="C19" t="n">
-        <v>23593</v>
+          <t>('MIN', 'MIN')</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>24092.79883337583</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>LAB</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>MAN</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
-        <v>959036.53</v>
+          <t>('MIN', 'MAN')</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>386766.2071966509</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>LAB</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>ESW</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
-        <v>92438</v>
+          <t>('MIN', 'ESW')</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>25400.93814486871</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>LAB</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>CON</t>
-        </is>
-      </c>
-      <c r="C22" t="n">
-        <v>576094</v>
+          <t>('MIN', 'CON')</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>30205.13465254084</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>LAB</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>WRT</t>
-        </is>
-      </c>
-      <c r="C23" t="n">
-        <v>975807</v>
+          <t>('MIN', 'WRT')</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>554.7138472670425</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>LAB</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>TRS</t>
-        </is>
-      </c>
-      <c r="C24" t="n">
-        <v>241220</v>
+          <t>('MIN', 'TRS')</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>60.33259108559908</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>LAB</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>AFS</t>
-        </is>
-      </c>
-      <c r="C25" t="n">
-        <v>127419</v>
+          <t>('MIN', 'AFS')</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>121.3883533638887</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>LAB</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>INF</t>
-        </is>
-      </c>
-      <c r="C26" t="n">
-        <v>156760</v>
+          <t>('MIN', 'INF')</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>44.76267229817115</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>LAB</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>FIN</t>
-        </is>
-      </c>
-      <c r="C27" t="n">
-        <v>427069</v>
+          <t>('MIN', 'FIN')</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>87.47359940953065</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>LAB</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>REA</t>
-        </is>
-      </c>
-      <c r="C28" t="n">
-        <v>56837</v>
+          <t>('MIN', 'REA')</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>619.7676712045622</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>LAB</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>PBS</t>
-        </is>
-      </c>
-      <c r="C29" t="n">
-        <v>725200</v>
+          <t>('MIN', 'PBS')</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>110.111208618299</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>LAB</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>PAD</t>
-        </is>
-      </c>
-      <c r="C30" t="n">
-        <v>612367</v>
+          <t>('MIN', 'PAD')</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>75.57409461921016</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>LAB</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>EDU</t>
-        </is>
-      </c>
-      <c r="C31" t="n">
-        <v>559598</v>
+          <t>('MIN', 'EDU')</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>40.98978434403799</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>LAB</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>HHS</t>
-        </is>
-      </c>
-      <c r="C32" t="n">
-        <v>84287</v>
+          <t>('MIN', 'HHS')</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>17.20957189616361</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>LAB</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>OTH</t>
-        </is>
-      </c>
-      <c r="C33" t="n">
-        <v>98666.46999999974</v>
+          <t>('MIN', 'OTH')</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>28.85883731522917</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>('MAN', 'AGR')</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>562317.1813914984</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>('MAN', 'MIN')</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>32889.50558041631</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>('MAN', 'MAN')</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>3536384.555394445</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>('MAN', 'ESW')</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>169840.3628270353</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>('MAN', 'CON')</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>1185357.660552872</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>('MAN', 'WRT')</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>159824.3694267376</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>('MAN', 'TRS')</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>421376.2451161093</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>('MAN', 'AFS')</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>232131.569601793</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>('MAN', 'INF')</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>128836.3952206124</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>('MAN', 'FIN')</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>94652.76397187269</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>('MAN', 'REA')</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>43047.18661193399</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>('MAN', 'PBS')</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>127914.3668898133</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>('MAN', 'PAD')</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>25993.78164756393</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>('MAN', 'EDU')</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>38145.22126086871</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>('MAN', 'HHS')</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>32035.35572329106</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>('MAN', 'OTH')</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>53452.78309609117</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>('ESW', 'AGR')</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>23680.12450086494</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>('ESW', 'MIN')</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>4258.121092261274</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>('ESW', 'MAN')</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>251159.6278232176</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>('ESW', 'ESW')</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>38201.89914724839</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>('ESW', 'CON')</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>41069.58495758228</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>('ESW', 'WRT')</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>68364.54647427362</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>('ESW', 'TRS')</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>29101.75632494179</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>('ESW', 'AFS')</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>14559.03440803147</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>('ESW', 'INF')</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>23427.48332184359</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>('ESW', 'FIN')</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>46150.93133109502</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>('ESW', 'REA')</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>21759.37696278335</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>('ESW', 'PBS')</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>46542.62425884105</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>('ESW', 'PAD')</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>7503.299767465179</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>('ESW', 'EDU')</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>7286.174502210705</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>('ESW', 'HHS')</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>7097.341416109978</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>('ESW', 'OTH')</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>7416.897539297385</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>('CON', 'AGR')</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>224.7272828615001</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>('CON', 'MIN')</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>173.8153879829501</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>('CON', 'MAN')</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>4996.512834695077</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>('CON', 'ESW')</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>276.6235712497684</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>('CON', 'CON')</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>1232.245435416442</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>('CON', 'WRT')</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>5856.068227410703</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>('CON', 'TRS')</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>2040.773234874782</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>('CON', 'AFS')</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>1134.678551830647</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>('CON', 'INF')</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>4263.535655062377</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>('CON', 'FIN')</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>2782.808024353337</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>('CON', 'REA')</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>316.9983391350282</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>('CON', 'PBS')</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>14455.75492983291</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>('CON', 'PAD')</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>206.9246343398124</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>('CON', 'EDU')</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>130.9767888995716</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>('CON', 'HHS')</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>912.0891916591041</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>('CON', 'OTH')</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>338.63275475275</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>('WRT', 'AGR')</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>36797.3558384009</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>('WRT', 'MIN')</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>5431.789807406018</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>('WRT', 'MAN')</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>1083840.331624043</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>('WRT', 'ESW')</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>36567.36673926556</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>('WRT', 'CON')</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>176115.7238993268</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>('WRT', 'WRT')</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>629355.3653459012</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>('WRT', 'TRS')</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>50782.20817613851</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>('WRT', 'AFS')</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>180339.3673151789</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>('WRT', 'INF')</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>40468.48989345161</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>('WRT', 'FIN')</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>79355.15029333404</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>('WRT', 'REA')</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>45911.62510533771</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>('WRT', 'PBS')</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>104995.5931434584</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>('WRT', 'PAD')</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>43593.4829173751</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>('WRT', 'EDU')</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>24589.96981740024</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>('WRT', 'HHS')</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>22665.76219802206</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>('WRT', 'OTH')</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>40428.24116361269</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>('TRS', 'AGR')</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
+        <v>17531.40922853843</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>('TRS', 'MIN')</t>
+        </is>
+      </c>
+      <c r="B99" t="n">
+        <v>3349.304543958308</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>('TRS', 'MAN')</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
+        <v>195974.6734952563</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>('TRS', 'ESW')</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>2724.247464785552</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>('TRS', 'CON')</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>18679.52557679249</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>('TRS', 'WRT')</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>118620.5156491477</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>('TRS', 'TRS')</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>273817.9512093465</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>('TRS', 'AFS')</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>9177.580968609169</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>('TRS', 'INF')</t>
+        </is>
+      </c>
+      <c r="B106" t="n">
+        <v>33246.43879831057</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>('TRS', 'FIN')</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>5642.141361711995</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>('TRS', 'REA')</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>14363.30388731421</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>('TRS', 'PBS')</t>
+        </is>
+      </c>
+      <c r="B109" t="n">
+        <v>25390.47786541112</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>('TRS', 'PAD')</t>
+        </is>
+      </c>
+      <c r="B110" t="n">
+        <v>22661.60505308602</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>('TRS', 'EDU')</t>
+        </is>
+      </c>
+      <c r="B111" t="n">
+        <v>4451.960926071457</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>('TRS', 'HHS')</t>
+        </is>
+      </c>
+      <c r="B112" t="n">
+        <v>1068.949165803444</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>('TRS', 'OTH')</t>
+        </is>
+      </c>
+      <c r="B113" t="n">
+        <v>887.9321545985744</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>('AFS', 'AGR')</t>
+        </is>
+      </c>
+      <c r="B114" t="n">
+        <v>190.5485593842953</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>('AFS', 'MIN')</t>
+        </is>
+      </c>
+      <c r="B115" t="n">
+        <v>31.68824515194521</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>('AFS', 'MAN')</t>
+        </is>
+      </c>
+      <c r="B116" t="n">
+        <v>4123.192252520734</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>('AFS', 'ESW')</t>
+        </is>
+      </c>
+      <c r="B117" t="n">
+        <v>170.525831571405</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>('AFS', 'CON')</t>
+        </is>
+      </c>
+      <c r="B118" t="n">
+        <v>657.5077035740391</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>('AFS', 'WRT')</t>
+        </is>
+      </c>
+      <c r="B119" t="n">
+        <v>2161.22177472801</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>('AFS', 'TRS')</t>
+        </is>
+      </c>
+      <c r="B120" t="n">
+        <v>1554.140067831092</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>('AFS', 'AFS')</t>
+        </is>
+      </c>
+      <c r="B121" t="n">
+        <v>129651.1464599214</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>('AFS', 'INF')</t>
+        </is>
+      </c>
+      <c r="B122" t="n">
+        <v>863.7331225685518</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>('AFS', 'FIN')</t>
+        </is>
+      </c>
+      <c r="B123" t="n">
+        <v>3906.237028514126</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>('AFS', 'REA')</t>
+        </is>
+      </c>
+      <c r="B124" t="n">
+        <v>233.7506847980509</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>('AFS', 'PBS')</t>
+        </is>
+      </c>
+      <c r="B125" t="n">
+        <v>2384.908631432158</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>('AFS', 'PAD')</t>
+        </is>
+      </c>
+      <c r="B126" t="n">
+        <v>14131.62372138642</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>('AFS', 'EDU')</t>
+        </is>
+      </c>
+      <c r="B127" t="n">
+        <v>141.2260852838927</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>('AFS', 'HHS')</t>
+        </is>
+      </c>
+      <c r="B128" t="n">
+        <v>454.224649948026</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>('AFS', 'OTH')</t>
+        </is>
+      </c>
+      <c r="B129" t="n">
+        <v>2015.03857679833</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>('INF', 'AGR')</t>
+        </is>
+      </c>
+      <c r="B130" t="n">
+        <v>10089.9896440092</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>('INF', 'MIN')</t>
+        </is>
+      </c>
+      <c r="B131" t="n">
+        <v>1033.763083661777</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>('INF', 'MAN')</t>
+        </is>
+      </c>
+      <c r="B132" t="n">
+        <v>87400.57085120806</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>('INF', 'ESW')</t>
+        </is>
+      </c>
+      <c r="B133" t="n">
+        <v>6409.948712335483</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>('INF', 'CON')</t>
+        </is>
+      </c>
+      <c r="B134" t="n">
+        <v>16821.84852122067</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>('INF', 'WRT')</t>
+        </is>
+      </c>
+      <c r="B135" t="n">
+        <v>33324.55059423266</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>('INF', 'TRS')</t>
+        </is>
+      </c>
+      <c r="B136" t="n">
+        <v>16030.92241827518</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>('INF', 'AFS')</t>
+        </is>
+      </c>
+      <c r="B137" t="n">
+        <v>8767.879875138795</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>('INF', 'INF')</t>
+        </is>
+      </c>
+      <c r="B138" t="n">
+        <v>52028.20605016277</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>('INF', 'FIN')</t>
+        </is>
+      </c>
+      <c r="B139" t="n">
+        <v>35141.4421327932</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>('INF', 'REA')</t>
+        </is>
+      </c>
+      <c r="B140" t="n">
+        <v>22237.90806269026</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>('INF', 'PBS')</t>
+        </is>
+      </c>
+      <c r="B141" t="n">
+        <v>23949.54476326111</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>('INF', 'PAD')</t>
+        </is>
+      </c>
+      <c r="B142" t="n">
+        <v>37082.79537782534</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>('INF', 'EDU')</t>
+        </is>
+      </c>
+      <c r="B143" t="n">
+        <v>4070.394710307927</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>('INF', 'HHS')</t>
+        </is>
+      </c>
+      <c r="B144" t="n">
+        <v>4276.69932878695</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>('INF', 'OTH')</t>
+        </is>
+      </c>
+      <c r="B145" t="n">
+        <v>4302.918261308165</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>('FIN', 'AGR')</t>
+        </is>
+      </c>
+      <c r="B146" t="n">
+        <v>29965.6972786291</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>('FIN', 'MIN')</t>
+        </is>
+      </c>
+      <c r="B147" t="n">
+        <v>3375.075360705922</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>('FIN', 'MAN')</t>
+        </is>
+      </c>
+      <c r="B148" t="n">
+        <v>280657.780433469</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>('FIN', 'ESW')</t>
+        </is>
+      </c>
+      <c r="B149" t="n">
+        <v>31702.75958278121</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>('FIN', 'CON')</t>
+        </is>
+      </c>
+      <c r="B150" t="n">
+        <v>87687.13267621709</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>('FIN', 'WRT')</t>
+        </is>
+      </c>
+      <c r="B151" t="n">
+        <v>108470.3227140286</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>('FIN', 'TRS')</t>
+        </is>
+      </c>
+      <c r="B152" t="n">
+        <v>54041.78996625963</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>('FIN', 'AFS')</t>
+        </is>
+      </c>
+      <c r="B153" t="n">
+        <v>10616.88118288948</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>('FIN', 'INF')</t>
+        </is>
+      </c>
+      <c r="B154" t="n">
+        <v>39079.32421015717</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>('FIN', 'FIN')</t>
+        </is>
+      </c>
+      <c r="B155" t="n">
+        <v>544109.0187771801</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>('FIN', 'REA')</t>
+        </is>
+      </c>
+      <c r="B156" t="n">
+        <v>63852.75474085637</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>('FIN', 'PBS')</t>
+        </is>
+      </c>
+      <c r="B157" t="n">
+        <v>74920.82107145021</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>('FIN', 'PAD')</t>
+        </is>
+      </c>
+      <c r="B158" t="n">
+        <v>117868.7463496854</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>('FIN', 'EDU')</t>
+        </is>
+      </c>
+      <c r="B159" t="n">
+        <v>14279.81208682949</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>('FIN', 'HHS')</t>
+        </is>
+      </c>
+      <c r="B160" t="n">
+        <v>15635.81331660888</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>('FIN', 'OTH')</t>
+        </is>
+      </c>
+      <c r="B161" t="n">
+        <v>10995.11004725444</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>('REA', 'AGR')</t>
+        </is>
+      </c>
+      <c r="B162" t="n">
+        <v>9387.562623335931</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>('REA', 'MIN')</t>
+        </is>
+      </c>
+      <c r="B163" t="n">
+        <v>4251.761191120128</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>('REA', 'MAN')</t>
+        </is>
+      </c>
+      <c r="B164" t="n">
+        <v>131850.0203817157</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>('REA', 'ESW')</t>
+        </is>
+      </c>
+      <c r="B165" t="n">
+        <v>7026.402470984634</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>('REA', 'CON')</t>
+        </is>
+      </c>
+      <c r="B166" t="n">
+        <v>2414.365692738618</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>('REA', 'WRT')</t>
+        </is>
+      </c>
+      <c r="B167" t="n">
+        <v>212606.6136742881</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>('REA', 'TRS')</t>
+        </is>
+      </c>
+      <c r="B168" t="n">
+        <v>36242.20451189306</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>('REA', 'AFS')</t>
+        </is>
+      </c>
+      <c r="B169" t="n">
+        <v>23664.4564037997</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>('REA', 'INF')</t>
+        </is>
+      </c>
+      <c r="B170" t="n">
+        <v>82034.16324574809</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>('REA', 'FIN')</t>
+        </is>
+      </c>
+      <c r="B171" t="n">
+        <v>148991.1948680506</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>('REA', 'REA')</t>
+        </is>
+      </c>
+      <c r="B172" t="n">
+        <v>63319.5053283951</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>('REA', 'PBS')</t>
+        </is>
+      </c>
+      <c r="B173" t="n">
+        <v>109936.0050247709</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>('REA', 'PAD')</t>
+        </is>
+      </c>
+      <c r="B174" t="n">
+        <v>9056.529986120127</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>('REA', 'EDU')</t>
+        </is>
+      </c>
+      <c r="B175" t="n">
+        <v>20009.95200306803</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>('REA', 'HHS')</t>
+        </is>
+      </c>
+      <c r="B176" t="n">
+        <v>16409.31651151967</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>('REA', 'OTH')</t>
+        </is>
+      </c>
+      <c r="B177" t="n">
+        <v>16860.76859074634</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>('PBS', 'AGR')</t>
+        </is>
+      </c>
+      <c r="B178" t="n">
+        <v>7671.725655247233</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>('PBS', 'MIN')</t>
+        </is>
+      </c>
+      <c r="B179" t="n">
+        <v>1198.499581918997</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>('PBS', 'MAN')</t>
+        </is>
+      </c>
+      <c r="B180" t="n">
+        <v>93942.00139192962</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>('PBS', 'ESW')</t>
+        </is>
+      </c>
+      <c r="B181" t="n">
+        <v>13290.59523430951</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>('PBS', 'CON')</t>
+        </is>
+      </c>
+      <c r="B182" t="n">
+        <v>54723.08811872249</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>('PBS', 'WRT')</t>
+        </is>
+      </c>
+      <c r="B183" t="n">
+        <v>41335.30632651814</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>('PBS', 'TRS')</t>
+        </is>
+      </c>
+      <c r="B184" t="n">
+        <v>131563.2974169935</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>('PBS', 'AFS')</t>
+        </is>
+      </c>
+      <c r="B185" t="n">
+        <v>41427.66918069134</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>('PBS', 'INF')</t>
+        </is>
+      </c>
+      <c r="B186" t="n">
+        <v>122915.7609529236</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>('PBS', 'FIN')</t>
+        </is>
+      </c>
+      <c r="B187" t="n">
+        <v>265714.1567284354</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>('PBS', 'REA')</t>
+        </is>
+      </c>
+      <c r="B188" t="n">
+        <v>54806.72631406299</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>('PBS', 'PBS')</t>
+        </is>
+      </c>
+      <c r="B189" t="n">
+        <v>280494.5109468997</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>('PBS', 'PAD')</t>
+        </is>
+      </c>
+      <c r="B190" t="n">
+        <v>10593.21682983673</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>('PBS', 'EDU')</t>
+        </is>
+      </c>
+      <c r="B191" t="n">
+        <v>5684.394091299144</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>('PBS', 'HHS')</t>
+        </is>
+      </c>
+      <c r="B192" t="n">
+        <v>28859.09469763844</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>('PBS', 'OTH')</t>
+        </is>
+      </c>
+      <c r="B193" t="n">
+        <v>10795.41906703843</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>('PAD', 'AGR')</t>
+        </is>
+      </c>
+      <c r="B194" t="n">
+        <v>130.3430781668181</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>('PAD', 'MIN')</t>
+        </is>
+      </c>
+      <c r="B195" t="n">
+        <v>59.17207945961287</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>('PAD', 'MAN')</t>
+        </is>
+      </c>
+      <c r="B196" t="n">
+        <v>1833.370805769428</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>('PAD', 'ESW')</t>
+        </is>
+      </c>
+      <c r="B197" t="n">
+        <v>285.6756973789712</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>('PAD', 'CON')</t>
+        </is>
+      </c>
+      <c r="B198" t="n">
+        <v>32.8274165087924</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>('PAD', 'WRT')</t>
+        </is>
+      </c>
+      <c r="B199" t="n">
+        <v>2959.766329414751</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>('PAD', 'TRS')</t>
+        </is>
+      </c>
+      <c r="B200" t="n">
+        <v>504.2821752044293</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>('PAD', 'AFS')</t>
+        </is>
+      </c>
+      <c r="B201" t="n">
+        <v>329.3262663006252</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>('PAD', 'INF')</t>
+        </is>
+      </c>
+      <c r="B202" t="n">
+        <v>1142.065415761599</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>('PAD', 'FIN')</t>
+        </is>
+      </c>
+      <c r="B203" t="n">
+        <v>2074.232428719989</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>('PAD', 'REA')</t>
+        </is>
+      </c>
+      <c r="B204" t="n">
+        <v>881.4898055408516</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>('PAD', 'PBS')</t>
+        </is>
+      </c>
+      <c r="B205" t="n">
+        <v>1530.181350854171</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>('PAD', 'PAD')</t>
+        </is>
+      </c>
+      <c r="B206" t="n">
+        <v>200553.4450487138</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>('PAD', 'EDU')</t>
+        </is>
+      </c>
+      <c r="B207" t="n">
+        <v>278.5757751426285</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>('PAD', 'HHS')</t>
+        </is>
+      </c>
+      <c r="B208" t="n">
+        <v>228.4063210516134</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>('PAD', 'OTH')</t>
+        </is>
+      </c>
+      <c r="B209" t="n">
+        <v>224.8375270473168</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>('EDU', 'AGR')</t>
+        </is>
+      </c>
+      <c r="B210" t="n">
+        <v>2778.315250756939</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>('EDU', 'MIN')</t>
+        </is>
+      </c>
+      <c r="B211" t="n">
+        <v>542.7758068847991</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>('EDU', 'MAN')</t>
+        </is>
+      </c>
+      <c r="B212" t="n">
+        <v>37061.93836946738</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>('EDU', 'ESW')</t>
+        </is>
+      </c>
+      <c r="B213" t="n">
+        <v>5019.468010577606</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>('EDU', 'CON')</t>
+        </is>
+      </c>
+      <c r="B214" t="n">
+        <v>11282.78686576815</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>('EDU', 'WRT')</t>
+        </is>
+      </c>
+      <c r="B215" t="n">
+        <v>15112.70997075617</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>('EDU', 'TRS')</t>
+        </is>
+      </c>
+      <c r="B216" t="n">
+        <v>18494.36720134626</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>('EDU', 'AFS')</t>
+        </is>
+      </c>
+      <c r="B217" t="n">
+        <v>2317.133481337426</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>('EDU', 'INF')</t>
+        </is>
+      </c>
+      <c r="B218" t="n">
+        <v>3727.739661860719</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>('EDU', 'FIN')</t>
+        </is>
+      </c>
+      <c r="B219" t="n">
+        <v>9138.766773565736</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>('EDU', 'REA')</t>
+        </is>
+      </c>
+      <c r="B220" t="n">
+        <v>6348.413799460275</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>('EDU', 'PBS')</t>
+        </is>
+      </c>
+      <c r="B221" t="n">
+        <v>26823.73566237933</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>('EDU', 'PAD')</t>
+        </is>
+      </c>
+      <c r="B222" t="n">
+        <v>3771.408181945571</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>('EDU', 'EDU')</t>
+        </is>
+      </c>
+      <c r="B223" t="n">
+        <v>1655.903869521936</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>('EDU', 'HHS')</t>
+        </is>
+      </c>
+      <c r="B224" t="n">
+        <v>7689.051612621561</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>('EDU', 'OTH')</t>
+        </is>
+      </c>
+      <c r="B225" t="n">
+        <v>2710.279428830022</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>('HHS', 'AGR')</t>
+        </is>
+      </c>
+      <c r="B226" t="n">
+        <v>325.8283497189743</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>('HHS', 'MIN')</t>
+        </is>
+      </c>
+      <c r="B227" t="n">
+        <v>51.47494382944985</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>('HHS', 'MAN')</t>
+        </is>
+      </c>
+      <c r="B228" t="n">
+        <v>6916.856511036302</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>('HHS', 'ESW')</t>
+        </is>
+      </c>
+      <c r="B229" t="n">
+        <v>369.233986241517</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>('HHS', 'CON')</t>
+        </is>
+      </c>
+      <c r="B230" t="n">
+        <v>1775.27247268218</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>('HHS', 'WRT')</t>
+        </is>
+      </c>
+      <c r="B231" t="n">
+        <v>5928.014601319257</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>('HHS', 'TRS')</t>
+        </is>
+      </c>
+      <c r="B232" t="n">
+        <v>1031.395597177054</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>('HHS', 'AFS')</t>
+        </is>
+      </c>
+      <c r="B233" t="n">
+        <v>1608.551307985471</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>('HHS', 'INF')</t>
+        </is>
+      </c>
+      <c r="B234" t="n">
+        <v>677.4327596080684</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>('HHS', 'FIN')</t>
+        </is>
+      </c>
+      <c r="B235" t="n">
+        <v>1698.715141718269</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>('HHS', 'REA')</t>
+        </is>
+      </c>
+      <c r="B236" t="n">
+        <v>645.5155124368843</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>('HHS', 'PBS')</t>
+        </is>
+      </c>
+      <c r="B237" t="n">
+        <v>1645.530889760532</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>('HHS', 'PAD')</t>
+        </is>
+      </c>
+      <c r="B238" t="n">
+        <v>761.9280649988186</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>('HHS', 'EDU')</t>
+        </is>
+      </c>
+      <c r="B239" t="n">
+        <v>537.7236817026917</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>('HHS', 'HHS')</t>
+        </is>
+      </c>
+      <c r="B240" t="n">
+        <v>11949.50026854712</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>('HHS', 'OTH')</t>
+        </is>
+      </c>
+      <c r="B241" t="n">
+        <v>386.8847934372729</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>('OTH', 'AGR')</t>
+        </is>
+      </c>
+      <c r="B242" t="n">
+        <v>1046.295292655768</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>('OTH', 'MIN')</t>
+        </is>
+      </c>
+      <c r="B243" t="n">
+        <v>130.1836001021431</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>('OTH', 'MAN')</t>
+        </is>
+      </c>
+      <c r="B244" t="n">
+        <v>11809.09997807655</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>('OTH', 'ESW')</t>
+        </is>
+      </c>
+      <c r="B245" t="n">
+        <v>825.7796476708539</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>('OTH', 'CON')</t>
+        </is>
+      </c>
+      <c r="B246" t="n">
+        <v>3297.724954117424</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>('OTH', 'WRT')</t>
+        </is>
+      </c>
+      <c r="B247" t="n">
+        <v>11905.56344431094</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>('OTH', 'TRS')</t>
+        </is>
+      </c>
+      <c r="B248" t="n">
+        <v>2030.975650240378</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>('OTH', 'AFS')</t>
+        </is>
+      </c>
+      <c r="B249" t="n">
+        <v>7229.999439492259</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>('OTH', 'INF')</t>
+        </is>
+      </c>
+      <c r="B250" t="n">
+        <v>1917.548880912487</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>('OTH', 'FIN')</t>
+        </is>
+      </c>
+      <c r="B251" t="n">
+        <v>5140.148725132723</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>('OTH', 'REA')</t>
+        </is>
+      </c>
+      <c r="B252" t="n">
+        <v>1583.233059004502</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>('OTH', 'PBS')</t>
+        </is>
+      </c>
+      <c r="B253" t="n">
+        <v>5884.108741303054</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>('OTH', 'PAD')</t>
+        </is>
+      </c>
+      <c r="B254" t="n">
+        <v>1109.271824274989</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>('OTH', 'EDU')</t>
+        </is>
+      </c>
+      <c r="B255" t="n">
+        <v>3763.941165659353</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>('OTH', 'HHS')</t>
+        </is>
+      </c>
+      <c r="B256" t="n">
+        <v>1794.712358636747</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>('OTH', 'OTH')</t>
+        </is>
+      </c>
+      <c r="B257" t="n">
+        <v>30230.98358170662</v>
       </c>
     </row>
   </sheetData>

</xml_diff>